<commit_message>
Mise à jour dashboard
Changement du Excel en raison de commentaires de la GIRE + test du script "RUN_BUILD.bat" en parallèle. Tout semble fonctionner.
</commit_message>
<xml_diff>
--- a/suivi-des-objectifs_OBVFSJ.xlsx
+++ b/suivi-des-objectifs_OBVFSJ.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="280">
   <si>
     <t>OBV</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Date d’extraction</t>
   </si>
   <si>
-    <t>14-01-2026</t>
+    <t>19-01-2026</t>
   </si>
   <si>
     <t>Année financière</t>
@@ -261,6 +261,9 @@
     <t>Recensement du nombre de municipalités formées</t>
   </si>
   <si>
+    <t>Pas d'avancement pour l'instant, valeur de référence inscrite.</t>
+  </si>
+  <si>
     <t>D'ici 2034, mener 5 campagnes de sensibilisation auprès des jeunes sur les enjeux liés à la qualité de l'eau à l'échelle de la ZGIEBV</t>
   </si>
   <si>
@@ -444,18 +447,18 @@
     <t>Voir actions 2.1.9, 2.1.10, 2.1.11</t>
   </si>
   <si>
-    <t>D'ici 2034, mettre en place une offre de service-conseil auprès des propriétaires riverains à l'échelle de la ZGIEBV pour proposer des solutions de végétalisation des bandes riveraines</t>
+    <t>D’ici 2034, 20 propriétaires riverains ont bénéficié d’une offre de service-conseil à l'échelle de la ZGIEBV pour proposer des solutions de végétalisation des bandes riveraines.</t>
   </si>
   <si>
     <t>Nombre d'offres de service-conseil mises en place</t>
   </si>
   <si>
+    <t>Avoir bénéficié</t>
+  </si>
+  <si>
     <t>Recensement de l'offre de service-conseil auprès des propriétaires riverains</t>
   </si>
   <si>
-    <t>Le libellé de l'objectif changera grandement suite à l'approbation du PDE. L'offre de service-conseil est en train d'être développée au gré des projets de revégétalisation auxquels nous contribuons.</t>
-  </si>
-  <si>
     <t>D'ici 2034, développer 2 outils de communication sur le vieillissement prématuré des lacs dans l'ensemble de la ZGIEBV</t>
   </si>
   <si>
@@ -504,12 +507,18 @@
     <t>CRECA, Horizon nature, OBVFSJ</t>
   </si>
   <si>
+    <t>Pas d'avancement pour l'instant, valeur de référence inscrite. Quelques rencontres effectuées avec le groupement forestier du Témiscouata, mais insuffisant pour considérer cela comme une campagne de sensibilisation.</t>
+  </si>
+  <si>
     <t>D'ci 2034, mener 6 campagnes de sensibilisation auprès des agriculteurs pour favoriser les saines pratiques agroenvironnementales dans l'ensemble de la ZGIEBV</t>
   </si>
   <si>
     <t>Ferticonseil, Groupe de conseil agricole de la Côte-du-Sud, OBVFSJ</t>
   </si>
   <si>
+    <t>Pas d'avancement pour l'instant, valeur de référence inscrite. Relations de plus en plus structurées avec les représentants des producteurs agricoles, pas encore de campagne de sensibilisation à plus grande échelle.</t>
+  </si>
+  <si>
     <t>D'ici 2034, conduire 2 ateliers de concertation pour réfléchir à un aménagement durable du territoire dans l'ensemble de la ZGIEBV</t>
   </si>
   <si>
@@ -684,10 +693,10 @@
     <t>40.00%</t>
   </si>
   <si>
-    <t>Ajout des bassins versants du Lac de l'Est et de la Rivière Noire</t>
-  </si>
-  <si>
-    <t>D'ici 2034, 50 traverses de cours d'eau non conformes et problématiques sont restaurées par les partenaires de l'OBVFSJ dans la ZGIEBV</t>
+    <t>2 BV supplémentaires : Rivière Chimenticook (Lac de l'Est) et Rivière Noire (Kamouraska)</t>
+  </si>
+  <si>
+    <t>D'ici 2034, 50 traverses de cours d'eau non conformes ou problématiques sont restaurées par les partenaires de l'OBVFSJ dans la ZGIEBV</t>
   </si>
   <si>
     <t>Nombre de traverses de cours d'eau non conformes et problématiques restaurées</t>
@@ -751,6 +760,9 @@
   </si>
   <si>
     <t>Recensement du nombre de nouveaux propriétaires mobilisés</t>
+  </si>
+  <si>
+    <t>Pas d'avancement pour l'instant, valeur de référence inscrite. Travail d'Horizon-Nature et CRECA à cet effet, il y aura un avancement à la fin 2026.</t>
   </si>
   <si>
     <t>D'ici 2034, participer à 10 évènements sur la protection du territoire dans la ZGIEBV</t>
@@ -2006,6 +2018,9 @@
       <c r="AB7" t="s">
         <v>54</v>
       </c>
+      <c r="AC7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="1" t="s">
@@ -2021,7 +2036,7 @@
         <v>1.14</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
         <v>71</v>
@@ -2075,10 +2090,10 @@
         <v>3</v>
       </c>
       <c r="AB8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AC8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -2089,22 +2104,22 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D9" s="1">
         <v>1.15</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G9" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I9" t="s">
         <v>47</v>
@@ -2134,7 +2149,7 @@
         <v>50</v>
       </c>
       <c r="S9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W9" t="s">
         <v>50</v>
@@ -2149,10 +2164,10 @@
         <v>1</v>
       </c>
       <c r="AB9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AC9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -2169,10 +2184,10 @@
         <v>1.2</v>
       </c>
       <c r="E10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
@@ -2208,10 +2223,10 @@
         <v>50</v>
       </c>
       <c r="S10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="T10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="W10" t="s">
         <v>50</v>
@@ -2226,10 +2241,10 @@
         <v>16</v>
       </c>
       <c r="AB10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AC10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -2246,10 +2261,10 @@
         <v>1.3</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G11" t="s">
         <v>45</v>
@@ -2285,7 +2300,7 @@
         <v>50</v>
       </c>
       <c r="S11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="W11" t="s">
         <v>50</v>
@@ -2303,7 +2318,7 @@
         <v>54</v>
       </c>
       <c r="AC11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -2320,19 +2335,19 @@
         <v>1.4</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G12" t="s">
         <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J12">
         <v>4</v>
@@ -2350,7 +2365,7 @@
         <v>9</v>
       </c>
       <c r="P12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>49</v>
@@ -2359,7 +2374,7 @@
         <v>50</v>
       </c>
       <c r="S12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="W12" t="s">
         <v>50</v>
@@ -2375,6 +2390,9 @@
       </c>
       <c r="AB12" t="s">
         <v>54</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -2391,19 +2409,19 @@
         <v>1.5</v>
       </c>
       <c r="E13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
         <v>45</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J13">
         <v>13</v>
@@ -2421,19 +2439,19 @@
         <v>54</v>
       </c>
       <c r="P13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="R13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="S13" t="s">
+        <v>114</v>
+      </c>
+      <c r="W13" t="s">
         <v>113</v>
-      </c>
-      <c r="W13" t="s">
-        <v>112</v>
       </c>
       <c r="X13" t="s">
         <v>52</v>
@@ -2445,10 +2463,10 @@
         <v>3</v>
       </c>
       <c r="AB13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AC13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -2465,19 +2483,19 @@
         <v>1.6</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G14" t="s">
         <v>45</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I14" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J14">
         <v>41</v>
@@ -2495,19 +2513,19 @@
         <v>54</v>
       </c>
       <c r="P14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="R14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="S14" t="s">
+        <v>123</v>
+      </c>
+      <c r="W14" t="s">
         <v>122</v>
-      </c>
-      <c r="W14" t="s">
-        <v>121</v>
       </c>
       <c r="X14" t="s">
         <v>52</v>
@@ -2522,7 +2540,7 @@
         <v>54</v>
       </c>
       <c r="AC14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:29">
@@ -2539,7 +2557,7 @@
         <v>1.7</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F15" t="s">
         <v>71</v>
@@ -2569,7 +2587,7 @@
         <v>20</v>
       </c>
       <c r="P15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>49</v>
@@ -2594,6 +2612,9 @@
       </c>
       <c r="AB15" t="s">
         <v>54</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -2610,16 +2631,16 @@
         <v>1.8</v>
       </c>
       <c r="E16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G16" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I16" t="s">
         <v>47</v>
@@ -2640,7 +2661,7 @@
         <v>5</v>
       </c>
       <c r="P16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>49</v>
@@ -2649,7 +2670,7 @@
         <v>50</v>
       </c>
       <c r="S16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="W16" t="s">
         <v>50</v>
@@ -2665,6 +2686,9 @@
       </c>
       <c r="AB16" t="s">
         <v>54</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:29">
@@ -2675,22 +2699,22 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1">
         <v>1.9</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I17" t="s">
         <v>47</v>
@@ -2720,7 +2744,7 @@
         <v>50</v>
       </c>
       <c r="S17" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W17" t="s">
         <v>50</v>
@@ -2738,27 +2762,27 @@
         <v>54</v>
       </c>
       <c r="AC17" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="1">
         <v>2.1</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G18" t="s">
         <v>45</v>
@@ -2794,7 +2818,7 @@
         <v>50</v>
       </c>
       <c r="S18" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="W18" t="s">
         <v>50</v>
@@ -2809,42 +2833,42 @@
         <v>3</v>
       </c>
       <c r="AB18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AC18" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1">
         <v>2.2</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G19" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="I19" t="s">
         <v>47</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="L19" t="s">
         <v>48</v>
@@ -2856,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="P19" t="s">
         <v>49</v>
@@ -2868,7 +2892,7 @@
         <v>50</v>
       </c>
       <c r="S19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="W19" t="s">
         <v>50</v>
@@ -2886,15 +2910,15 @@
         <v>54</v>
       </c>
       <c r="AC19" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
         <v>56</v>
@@ -2903,7 +2927,7 @@
         <v>2.3</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F20" t="s">
         <v>65</v>
@@ -2960,15 +2984,15 @@
         <v>68</v>
       </c>
       <c r="AC20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
         <v>56</v>
@@ -2977,10 +3001,10 @@
         <v>2.4</v>
       </c>
       <c r="E21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G21" t="s">
         <v>45</v>
@@ -3016,7 +3040,7 @@
         <v>50</v>
       </c>
       <c r="S21" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="W21" t="s">
         <v>50</v>
@@ -3034,15 +3058,15 @@
         <v>79</v>
       </c>
       <c r="AC21" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
         <v>56</v>
@@ -3051,7 +3075,7 @@
         <v>2.5</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F22" t="s">
         <v>71</v>
@@ -3099,24 +3123,24 @@
         <v>52</v>
       </c>
       <c r="Z22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA22">
         <v>1</v>
       </c>
       <c r="AB22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AC22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
         <v>56</v>
@@ -3125,16 +3149,16 @@
         <v>2.6</v>
       </c>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F23" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G23" t="s">
         <v>45</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I23" t="s">
         <v>47</v>
@@ -3164,7 +3188,7 @@
         <v>50</v>
       </c>
       <c r="S23" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="W23" t="s">
         <v>50</v>
@@ -3173,7 +3197,7 @@
         <v>52</v>
       </c>
       <c r="Z23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -3182,15 +3206,15 @@
         <v>54</v>
       </c>
       <c r="AC23" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
         <v>56</v>
@@ -3199,7 +3223,7 @@
         <v>2.7</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F24" t="s">
         <v>71</v>
@@ -3229,7 +3253,7 @@
         <v>6</v>
       </c>
       <c r="P24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>49</v>
@@ -3247,21 +3271,24 @@
         <v>52</v>
       </c>
       <c r="Z24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA24">
         <v>0</v>
       </c>
       <c r="AB24" t="s">
         <v>54</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
@@ -3270,7 +3297,7 @@
         <v>2.8</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F25" t="s">
         <v>71</v>
@@ -3300,7 +3327,7 @@
         <v>6</v>
       </c>
       <c r="P25" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>49</v>
@@ -3318,21 +3345,24 @@
         <v>52</v>
       </c>
       <c r="Z25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA25">
         <v>0</v>
       </c>
       <c r="AB25" t="s">
         <v>54</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
         <v>42</v>
@@ -3341,16 +3371,16 @@
         <v>2.9</v>
       </c>
       <c r="E26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F26" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G26" t="s">
         <v>45</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I26" t="s">
         <v>47</v>
@@ -3380,7 +3410,7 @@
         <v>50</v>
       </c>
       <c r="S26" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="W26" t="s">
         <v>50</v>
@@ -3389,7 +3419,7 @@
         <v>52</v>
       </c>
       <c r="Z26" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AA26">
         <v>0</v>
@@ -3398,15 +3428,15 @@
         <v>54</v>
       </c>
       <c r="AC26" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C27" t="s">
         <v>42</v>
@@ -3415,10 +3445,10 @@
         <v>3.1</v>
       </c>
       <c r="E27" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F27" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G27" t="s">
         <v>45</v>
@@ -3445,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="P27" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>49</v>
@@ -3454,7 +3484,7 @@
         <v>50</v>
       </c>
       <c r="S27" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="W27" t="s">
         <v>50</v>
@@ -3463,10 +3493,10 @@
         <v>52</v>
       </c>
       <c r="Y27" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="Z27" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA27">
         <v>1</v>
@@ -3475,15 +3505,15 @@
         <v>68</v>
       </c>
       <c r="AC27" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C28" t="s">
         <v>42</v>
@@ -3492,16 +3522,16 @@
         <v>3.2</v>
       </c>
       <c r="E28" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="F28" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G28" t="s">
         <v>45</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I28" t="s">
         <v>47</v>
@@ -3531,7 +3561,7 @@
         <v>50</v>
       </c>
       <c r="S28" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="W28" t="s">
         <v>50</v>
@@ -3540,45 +3570,45 @@
         <v>52</v>
       </c>
       <c r="Z28" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA28">
         <v>6</v>
       </c>
       <c r="AB28" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AC28" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1">
         <v>3.3</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F29" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
         <v>45</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I29" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="J29">
         <v>21</v>
@@ -3596,7 +3626,7 @@
         <v>26</v>
       </c>
       <c r="P29" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>49</v>
@@ -3605,7 +3635,7 @@
         <v>50</v>
       </c>
       <c r="S29" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="W29" t="s">
         <v>50</v>
@@ -3621,14 +3651,17 @@
       </c>
       <c r="AB29" t="s">
         <v>54</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C30" t="s">
         <v>56</v>
@@ -3637,7 +3670,7 @@
         <v>3.4</v>
       </c>
       <c r="E30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F30" t="s">
         <v>77</v>
@@ -3667,7 +3700,7 @@
         <v>54</v>
       </c>
       <c r="P30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>49</v>
@@ -3685,7 +3718,7 @@
         <v>52</v>
       </c>
       <c r="Z30" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA30">
         <v>0</v>
@@ -3694,15 +3727,15 @@
         <v>54</v>
       </c>
       <c r="AC30" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
         <v>56</v>
@@ -3711,10 +3744,10 @@
         <v>3.5</v>
       </c>
       <c r="E31" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F31" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G31" t="s">
         <v>45</v>
@@ -3750,7 +3783,7 @@
         <v>50</v>
       </c>
       <c r="S31" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="W31" t="s">
         <v>50</v>
@@ -3759,24 +3792,24 @@
         <v>52</v>
       </c>
       <c r="Z31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA31">
         <v>12</v>
       </c>
       <c r="AB31" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="AC31" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s">
         <v>56</v>
@@ -3785,7 +3818,7 @@
         <v>3.6</v>
       </c>
       <c r="E32" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F32" t="s">
         <v>71</v>
@@ -3824,7 +3857,7 @@
         <v>50</v>
       </c>
       <c r="S32" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="W32" t="s">
         <v>50</v>
@@ -3833,7 +3866,7 @@
         <v>52</v>
       </c>
       <c r="Z32" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA32">
         <v>2</v>
@@ -3842,15 +3875,15 @@
         <v>68</v>
       </c>
       <c r="AC32" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C33" t="s">
         <v>56</v>
@@ -3859,16 +3892,16 @@
         <v>3.7</v>
       </c>
       <c r="E33" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F33" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G33" t="s">
         <v>45</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I33" t="s">
         <v>47</v>
@@ -3898,7 +3931,7 @@
         <v>50</v>
       </c>
       <c r="S33" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="W33" t="s">
         <v>50</v>
@@ -3907,24 +3940,24 @@
         <v>52</v>
       </c>
       <c r="Z33" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA33">
         <v>3</v>
       </c>
       <c r="AB33" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AC33" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C34" t="s">
         <v>42</v>
@@ -3933,10 +3966,10 @@
         <v>4.1</v>
       </c>
       <c r="E34" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="G34" t="s">
         <v>45</v>
@@ -3963,7 +3996,7 @@
         <v>1</v>
       </c>
       <c r="P34" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>49</v>
@@ -3972,7 +4005,7 @@
         <v>50</v>
       </c>
       <c r="S34" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="W34" t="s">
         <v>50</v>
@@ -3981,21 +4014,24 @@
         <v>52</v>
       </c>
       <c r="Z34" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA34">
         <v>0</v>
       </c>
       <c r="AB34" t="s">
         <v>54</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
@@ -4004,16 +4040,16 @@
         <v>4.1</v>
       </c>
       <c r="E35" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F35" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G35" t="s">
         <v>45</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I35" t="s">
         <v>47</v>
@@ -4034,7 +4070,7 @@
         <v>5</v>
       </c>
       <c r="P35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>49</v>
@@ -4043,7 +4079,7 @@
         <v>50</v>
       </c>
       <c r="S35" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="W35" t="s">
         <v>50</v>
@@ -4052,21 +4088,24 @@
         <v>52</v>
       </c>
       <c r="Z35" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA35">
         <v>0</v>
       </c>
       <c r="AB35" t="s">
         <v>54</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C36" t="s">
         <v>42</v>
@@ -4075,16 +4114,16 @@
         <v>4.2</v>
       </c>
       <c r="E36" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F36" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G36" t="s">
         <v>45</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I36" t="s">
         <v>47</v>
@@ -4114,7 +4153,7 @@
         <v>50</v>
       </c>
       <c r="S36" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="W36" t="s">
         <v>50</v>
@@ -4123,21 +4162,24 @@
         <v>52</v>
       </c>
       <c r="Z36" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA36">
         <v>0</v>
       </c>
       <c r="AB36" t="s">
         <v>54</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
         <v>42</v>
@@ -4146,16 +4188,16 @@
         <v>4.3</v>
       </c>
       <c r="E37" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F37" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G37" t="s">
         <v>45</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I37" t="s">
         <v>47</v>
@@ -4185,10 +4227,10 @@
         <v>50</v>
       </c>
       <c r="S37" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="T37" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="W37" t="s">
         <v>50</v>
@@ -4197,42 +4239,42 @@
         <v>52</v>
       </c>
       <c r="Z37" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA37">
         <v>6</v>
       </c>
       <c r="AB37" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="AC37" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D38" s="1">
         <v>4.4</v>
       </c>
       <c r="E38" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G38" t="s">
         <v>45</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="I38" t="s">
         <v>47</v>
@@ -4253,7 +4295,7 @@
         <v>50</v>
       </c>
       <c r="P38" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>49</v>
@@ -4262,7 +4304,7 @@
         <v>50</v>
       </c>
       <c r="S38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="W38" t="s">
         <v>50</v>
@@ -4278,26 +4320,29 @@
       </c>
       <c r="AB38" t="s">
         <v>54</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D39" s="1">
         <v>4.5</v>
       </c>
       <c r="E39" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F39" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G39" t="s">
         <v>45</v>
@@ -4333,7 +4378,7 @@
         <v>50</v>
       </c>
       <c r="S39" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="W39" t="s">
         <v>50</v>
@@ -4342,7 +4387,7 @@
         <v>52</v>
       </c>
       <c r="Z39" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA39">
         <v>0</v>
@@ -4351,15 +4396,15 @@
         <v>54</v>
       </c>
       <c r="AC39" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
         <v>56</v>
@@ -4368,10 +4413,10 @@
         <v>4.6</v>
       </c>
       <c r="E40" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F40" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G40" t="s">
         <v>45</v>
@@ -4407,7 +4452,7 @@
         <v>50</v>
       </c>
       <c r="S40" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="W40" t="s">
         <v>50</v>
@@ -4416,7 +4461,7 @@
         <v>52</v>
       </c>
       <c r="Z40" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA40">
         <v>2</v>
@@ -4425,15 +4470,15 @@
         <v>68</v>
       </c>
       <c r="AC40" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s">
         <v>56</v>
@@ -4442,7 +4487,7 @@
         <v>4.7</v>
       </c>
       <c r="E41" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F41" t="s">
         <v>71</v>
@@ -4481,7 +4526,7 @@
         <v>50</v>
       </c>
       <c r="S41" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="W41" t="s">
         <v>50</v>
@@ -4490,24 +4535,24 @@
         <v>52</v>
       </c>
       <c r="Z41" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA41">
         <v>3</v>
       </c>
       <c r="AB41" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="AC41" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C42" t="s">
         <v>56</v>
@@ -4516,16 +4561,16 @@
         <v>4.8</v>
       </c>
       <c r="E42" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F42" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G42" t="s">
         <v>45</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I42" t="s">
         <v>47</v>
@@ -4546,7 +4591,7 @@
         <v>50</v>
       </c>
       <c r="P42" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="Q42" s="1" t="s">
         <v>49</v>
@@ -4555,7 +4600,7 @@
         <v>50</v>
       </c>
       <c r="S42" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="W42" t="s">
         <v>50</v>
@@ -4571,14 +4616,17 @@
       </c>
       <c r="AB42" t="s">
         <v>54</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C43" t="s">
         <v>56</v>
@@ -4587,16 +4635,16 @@
         <v>4.9</v>
       </c>
       <c r="E43" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="F43" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="G43" t="s">
         <v>45</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I43" t="s">
         <v>47</v>
@@ -4626,7 +4674,7 @@
         <v>50</v>
       </c>
       <c r="S43" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="W43" t="s">
         <v>50</v>
@@ -4635,7 +4683,7 @@
         <v>52</v>
       </c>
       <c r="Z43" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA43">
         <v>5</v>
@@ -4644,15 +4692,15 @@
         <v>79</v>
       </c>
       <c r="AC43" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C44" t="s">
         <v>42</v>
@@ -4661,16 +4709,16 @@
         <v>5.1</v>
       </c>
       <c r="E44" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F44" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="G44" t="s">
         <v>45</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I44" t="s">
         <v>47</v>
@@ -4691,7 +4739,7 @@
         <v>9</v>
       </c>
       <c r="P44" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>49</v>
@@ -4700,7 +4748,7 @@
         <v>50</v>
       </c>
       <c r="S44" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="W44" t="s">
         <v>50</v>
@@ -4709,21 +4757,24 @@
         <v>52</v>
       </c>
       <c r="Z44" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA44">
         <v>0</v>
       </c>
       <c r="AB44" t="s">
         <v>54</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C45" t="s">
         <v>42</v>
@@ -4732,16 +4783,16 @@
         <v>5.2</v>
       </c>
       <c r="E45" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F45" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="G45" t="s">
         <v>45</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="I45" t="s">
         <v>47</v>
@@ -4771,7 +4822,7 @@
         <v>50</v>
       </c>
       <c r="S45" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="W45" t="s">
         <v>50</v>
@@ -4780,24 +4831,24 @@
         <v>52</v>
       </c>
       <c r="Z45" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA45">
         <v>1</v>
       </c>
       <c r="AB45" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC45" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C46" t="s">
         <v>56</v>
@@ -4806,16 +4857,16 @@
         <v>5.3</v>
       </c>
       <c r="E46" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F46" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="G46" t="s">
         <v>45</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I46" t="s">
         <v>47</v>
@@ -4845,7 +4896,7 @@
         <v>50</v>
       </c>
       <c r="S46" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="W46" t="s">
         <v>50</v>
@@ -4854,42 +4905,42 @@
         <v>52</v>
       </c>
       <c r="Z46" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA46">
         <v>1</v>
       </c>
       <c r="AB46" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AC46" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D47" s="1">
         <v>5.4</v>
       </c>
       <c r="E47" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="F47" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G47" t="s">
         <v>45</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="I47" t="s">
         <v>47</v>
@@ -4919,7 +4970,7 @@
         <v>50</v>
       </c>
       <c r="S47" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="W47" t="s">
         <v>50</v>
@@ -4928,24 +4979,24 @@
         <v>52</v>
       </c>
       <c r="Z47" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA47">
         <v>1</v>
       </c>
       <c r="AB47" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="AC47" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C48" t="s">
         <v>56</v>
@@ -4954,7 +5005,7 @@
         <v>5.5</v>
       </c>
       <c r="E48" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="F48" t="s">
         <v>65</v>
@@ -4993,7 +5044,7 @@
         <v>50</v>
       </c>
       <c r="S48" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="W48" t="s">
         <v>50</v>
@@ -5002,7 +5053,7 @@
         <v>52</v>
       </c>
       <c r="Z48" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA48">
         <v>1</v>
@@ -5011,15 +5062,15 @@
         <v>79</v>
       </c>
       <c r="AC48" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:29">
       <c r="A49" s="1" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C49" t="s">
         <v>56</v>
@@ -5028,7 +5079,7 @@
         <v>5.6</v>
       </c>
       <c r="E49" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F49" t="s">
         <v>71</v>
@@ -5067,7 +5118,7 @@
         <v>50</v>
       </c>
       <c r="S49" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="W49" t="s">
         <v>50</v>
@@ -5076,7 +5127,7 @@
         <v>52</v>
       </c>
       <c r="Z49" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AA49">
         <v>1</v>
@@ -5085,7 +5136,7 @@
         <v>79</v>
       </c>
       <c r="AC49" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>